<commit_message>
Fully implemented core functionalities
- Implemented expense tracking (add/view/delete)
- Completed expenses page with chart visualization
- Polished UI for consistency and responsiveness
- Cleaned up and reorganized components
- Project is ready for initial deployment

TODO: Deploy v1 of the expense tracker
</commit_message>
<xml_diff>
--- a/backend/expense.xlsx
+++ b/backend/expense.xlsx
@@ -398,14 +398,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Category</v>
+        <v>Description</v>
       </c>
       <c r="B1" t="str">
         <v>Amount</v>
@@ -416,18 +416,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Groceries</v>
+        <v>Rent</v>
       </c>
       <c r="B2">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C2" s="1">
-        <v>45858.833333333336</v>
+        <v>45862</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Cat Food</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45861</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>